<commit_message>
tried to convert Exceptions.xlsx. to pdf
</commit_message>
<xml_diff>
--- a/BusinessExceptions.xlsx
+++ b/BusinessExceptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{0BC64655-0547-44AD-AD12-44843BF79323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2EC7CF35-0618-4E44-AA55-CBA759AC5333}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{0BC64655-0547-44AD-AD12-44843BF79323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0947C1E-C443-4DB9-9B1E-CDC65264EAB3}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{91D903ED-895F-495A-ADD1-5929788D1604}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{91D903ED-895F-495A-ADD1-5929788D1604}"/>
   </bookViews>
   <sheets>
     <sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="2">
   <si>
     <t>text</t>
   </si>
@@ -391,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DB9F82-8E33-46FB-805E-1CCBCB58BAF2}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B63"/>
@@ -731,33 +731,312 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Business Exception logging.
</commit_message>
<xml_diff>
--- a/BusinessExceptions.xlsx
+++ b/BusinessExceptions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{0BC64655-0547-44AD-AD12-44843BF79323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A18275D-4790-479E-A4EA-BF90BE531A88}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9595B6D-782B-4347-982D-23479F488693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8964" xr2:uid="{91D903ED-895F-495A-ADD1-5929788D1604}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="25590" windowHeight="12660" xr2:uid="{91D903ED-895F-495A-ADD1-5929788D1604}"/>
   </bookViews>
   <sheets>
     <sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
@@ -34,12 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>text</t>
+    <t>CHANGES - SOX...eml on 01/24/2020 00:00:00 missing Server Name magic_qq_appl (Expected Server Name)</t>
   </si>
   <si>
-    <t xml:space="preserve">CHANGES - SOX...eml on (selected date) does not contain Server Name </t>
+    <t>CHANGES - SOX...eml on 01/24/2020 00:00:00 missing Server Name testps9023 (Expected Server Name)</t>
   </si>
 </sst>
 </file>
@@ -391,94 +391,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DB9F82-8E33-46FB-805E-1CCBCB58BAF2}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B63"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -493,7 +420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>